<commit_message>
changes to cf and ff
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2058" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{51A3BD8F-45B0-49FA-9478-4BEEAF84D39D}"/>
+  <xr:revisionPtr revIDLastSave="2081" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{06838ADF-5235-4C4E-A887-70D440659DD8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="333">
   <si>
     <t>Cause</t>
   </si>
@@ -1190,6 +1190,12 @@
   </si>
   <si>
     <t>protection_trip</t>
+  </si>
+  <si>
+    <t>inspection_groundline</t>
+  </si>
+  <si>
+    <t>inspection_protection</t>
   </si>
 </sst>
 </file>
@@ -3548,8 +3554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AV80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC29" sqref="AC29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -3986,7 +3992,7 @@
         <v>1</v>
       </c>
       <c r="T5" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U5" s="45">
         <v>0.8</v>
@@ -4758,7 +4764,7 @@
         <v>1</v>
       </c>
       <c r="T17" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U17" s="45">
         <v>0.8</v>
@@ -5211,7 +5217,7 @@
         <v>1</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U25" s="45">
         <v>0.8</v>
@@ -5845,7 +5851,7 @@
       <c r="R36" s="41"/>
       <c r="S36" s="99"/>
       <c r="T36" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U36" s="15">
         <v>0.99</v>
@@ -5969,7 +5975,7 @@
       <c r="R38" s="15"/>
       <c r="S38" s="97"/>
       <c r="T38" s="15" t="s">
-        <v>79</v>
+        <v>332</v>
       </c>
       <c r="U38" s="15">
         <v>1</v>
@@ -6226,7 +6232,7 @@
       <c r="R42" s="15"/>
       <c r="S42" s="97"/>
       <c r="T42" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U42" s="15">
         <v>1</v>
@@ -6710,10 +6716,10 @@
         <v>1</v>
       </c>
       <c r="M50" s="41">
-        <v>50</v>
+        <v>161</v>
       </c>
       <c r="N50" s="41">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
       <c r="O50" s="134">
         <v>30</v>
@@ -6731,7 +6737,7 @@
         <v>2</v>
       </c>
       <c r="T50" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U50" s="15">
         <v>1</v>
@@ -7200,7 +7206,7 @@
       <c r="R58" s="15"/>
       <c r="S58" s="97"/>
       <c r="T58" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U58" s="15">
         <v>0.8</v>
@@ -7698,7 +7704,7 @@
       <c r="R66" s="15"/>
       <c r="S66" s="97"/>
       <c r="T66" s="15" t="s">
-        <v>79</v>
+        <v>331</v>
       </c>
       <c r="U66" s="15">
         <v>0.8</v>
@@ -8339,7 +8345,7 @@
       <c r="H80" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="AL13 B7:B13 X16:X17 U16:W16 C23:D23 E22:H23 B67:B70 B16:B23 C18:D20 E17:H19 C7:G7 T42:Y42 AG17:AN17 AD50:AQ50 AG25:AN25 AL23:AQ23 AL19:AQ20 AL40:AQ40 AL48:AQ48 AL56:AQ56 AN52:AQ53 AL44:AQ44 AL34:AQ34 AL30:AQ31 AO22:AV22 AO39:AQ39 AO17:AV18 AO47:AV47 AO55:AV55 AO51:AV51 AO43:AV43 AO33:AV33 AO25:AV29 AO37:AQ37 AR37:AV39 AO5:AV10 AL11:AV12 AL15:AV15 AO14:AV14 AL68:AV69 AO67:AV67 AL72:AV72 AO71:AV71 AL60:AV61 AO59:AV59 AL64:AV64 AO63:AV63 P36:Y36 P25:T25 P46:Y46 P12:S12 I7:O12 P37:S40 P48:S48 P52:S56 P71:S72 P61:S61 P34:S34 P29:S31 P76:U77 P15:V15 P24:W24 P27:Y27 B5:G6 I23:S23 I18:S20 C67:S69 B71:O77 C59:O61 B63:S64 I26:O31 C16:T17 B14:O15 C24:O25 AL38:AQ38 P42:S44 B35:H56 I34:O56 Z17:AC17 T22:AB22 T39:AB39 T18:AB18 T55:AB55 T43:AB43 T33:AB33 T71:AB71 T67:AB67 T37:AK37 T63:AB63 Y16:AU16 W76:AB77 Y24:AU24 AC10:AK11 P28:AB28 AC60:AF60 P14:AB14 P26:AK26 P59:AB60 AC59:AK59 AV59:AV60 AC8:AN9 P73:AB75 AC73:AU77 P35:AU35 P45:AU45 AC49:AU49 P41:AU41 P47:AB47 P7:AB11 AC7:AK7 B58:AV58 B66:AU66 I5:AN6 AV5:AV11 X15:AB15 AC14:AK15 AA36:AQ36 X19:AB19 AC18:AK19 AV14:AV19 AA46:AQ46 U23:AB23 AC22:AK23 U40:AB40 AC39:AK40 P49:AB51 U48:AB48 AC47:AK48 AA42:AQ42 T52:AB52 AC51:AK52 U56:AB56 AC55:AK56 AV55:AV56 U44:AB44 AC43:AK44 AA25:AC25 AA27:AB27 AC27:AN28 T29:AK30 AV22:AV30 U34:AB34 AC33:AK34 U68:AB68 AC67:AK68 AV66:AV68 U72:AB72 AC71:AK72 AV71:AV77 Z38:AC38 AV33:AV52 U64:AB64 AC63:AK64 AV63:AV64 C9:G12 C8:F8">
+  <conditionalFormatting sqref="AL13 B7:B13 X16:X17 U16:W16 C23:D23 E22:H23 B67:B70 B16:B23 C18:D20 E17:H19 C7:G7 AG17:AN17 AD50:AQ50 AG25:AN25 AL23:AQ23 AL19:AQ20 AL40:AQ40 AL48:AQ48 AL56:AQ56 AN52:AQ53 AL44:AQ44 AL34:AQ34 AL30:AQ31 AO22:AV22 AO39:AQ39 AO17:AV18 AO47:AV47 AO55:AV55 AO51:AV51 AO43:AV43 AO33:AV33 AO25:AV29 AO37:AQ37 AR37:AV39 AO5:AV10 AL11:AV12 AL15:AV15 AO14:AV14 AL68:AV69 AO67:AV67 AL72:AV72 AO71:AV71 AL60:AV61 AO59:AV59 AL64:AV64 AO63:AV63 P46:Y46 P12:S12 I7:O12 P37:S40 P48:S48 P52:S56 P71:S72 P61:S61 P34:S34 P29:S31 P76:U77 P15:V15 P24:W24 P27:Y27 B5:G6 I23:S23 I18:S20 C67:S69 B71:O77 C59:O61 B63:S64 I26:O31 B14:O15 C24:O25 AL38:AQ38 P42:S44 B35:H56 I34:O56 Z17:AC17 T22:AB22 T39:AB39 T18:AB18 T55:AB55 T43:AB43 T33:AB33 T71:AB71 T67:AB67 T37:AK37 T63:AB63 Y16:AU16 W76:AB77 Y24:AU24 AC10:AK11 P28:AB28 AC60:AF60 P14:AB14 P26:AK26 P59:AB60 AC59:AK59 AV59:AV60 AC8:AN9 P73:AB75 AC73:AU77 P35:AU35 P45:AU45 AC49:AU49 P41:AU41 P47:AB47 P7:AB11 AC7:AK7 I5:AN6 AV5:AV11 X15:AB15 AC14:AK15 AA36:AQ36 X19:AB19 AC18:AK19 AV14:AV19 AA46:AQ46 U23:AB23 AC22:AK23 U40:AB40 AC39:AK40 U48:AB48 AC47:AK48 AA42:AQ42 T52:AB52 AC51:AK52 U56:AB56 AC55:AK56 AV55:AV56 U44:AB44 AC43:AK44 AA25:AC25 AA27:AB27 AC27:AN28 T29:AK30 AV22:AV30 U34:AB34 AC33:AK34 U68:AB68 AC67:AK68 AV66:AV68 U72:AB72 AC71:AK72 AV71:AV77 Z38:AC38 AV33:AV52 U64:AB64 AC63:AK64 AV63:AV64 C9:G12 C8:F8 C16:T17 P25:T25 P36:Y36 T42:Y42 P49:AB51 B58:AV58 B66:AU66">
     <cfRule type="cellIs" dxfId="75" priority="182" operator="equal">
       <formula>"nil"</formula>
     </cfRule>

</xml_diff>

<commit_message>
small change to assetdata
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2126" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B4542127-864F-4278-876B-0405517AC208}"/>
+  <xr:revisionPtr revIDLastSave="2143" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4D04FE9A-11F1-4675-9A89-92153B46D92A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1333,7 +1333,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1463,6 +1463,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8CBAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -1509,7 +1515,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1787,6 +1793,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="4" builtinId="27"/>
@@ -3668,7 +3675,7 @@
   <dimension ref="A1:AV92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM20" sqref="AM20"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4070,8 +4077,9 @@
       <c r="G5" s="42">
         <v>125</v>
       </c>
-      <c r="H5" s="138">
-        <v>0</v>
+      <c r="H5" s="147">
+        <f>((H7 * G6^3)/(G7*8))^(1/3)</f>
+        <v>62.499999999999964</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>30</v>
@@ -4184,8 +4192,9 @@
       <c r="G6" s="42">
         <v>250</v>
       </c>
-      <c r="H6" s="138">
-        <v>0</v>
+      <c r="H6" s="147">
+        <f>(H7/G7 * G6^3)^(1/3)</f>
+        <v>124.99999999999994</v>
       </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>

</xml_diff>

<commit_message>
schedule task fix, condition indicator trigger fix
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2223" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{77DD6A1E-6213-462F-9F55-43C0B099A200}"/>
+  <xr:revisionPtr revIDLastSave="2234" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E6D1C31-637B-46AF-AB7E-E1D30A9F6E13}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="337">
   <si>
     <t>Cause</t>
   </si>
@@ -433,9 +433,6 @@
     <t>linear</t>
   </si>
   <si>
-    <t>termites _ cf</t>
-  </si>
-  <si>
     <t>inspection_groundline</t>
   </si>
   <si>
@@ -493,10 +490,10 @@
     <t>functional_failure</t>
   </si>
   <si>
-    <t>fungal decay _ external</t>
-  </si>
-  <si>
-    <t>fungal decay _ internal</t>
+    <t>fungal decay | external</t>
+  </si>
+  <si>
+    <t>fungal decay | internal</t>
   </si>
   <si>
     <t>pole_saver_rod</t>
@@ -2812,180 +2809,180 @@
   <sheetData>
     <row r="3" spans="1:19">
       <c r="A3" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" t="s">
         <v>269</v>
-      </c>
-      <c r="F3" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="F5" t="s">
         <v>271</v>
-      </c>
-      <c r="F5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
+        <v>272</v>
+      </c>
+      <c r="N6" t="s">
         <v>273</v>
-      </c>
-      <c r="N6" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="O12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="S12" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:19">
       <c r="F13" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="O13" t="s">
         <v>279</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
+        <v>170</v>
+      </c>
+      <c r="S13" t="s">
         <v>280</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>171</v>
-      </c>
-      <c r="S13" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:19">
       <c r="F14" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="O14" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q14" t="s">
         <v>282</v>
       </c>
-      <c r="O14" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="S14" t="s">
         <v>283</v>
-      </c>
-      <c r="S14" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:19">
       <c r="F15" t="s">
+        <v>284</v>
+      </c>
+      <c r="J15" t="s">
         <v>285</v>
       </c>
-      <c r="J15" t="s">
+      <c r="O15" t="s">
         <v>286</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>287</v>
       </c>
-      <c r="Q15" t="s">
-        <v>288</v>
-      </c>
       <c r="S15" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:19">
       <c r="F16" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>97</v>
+      </c>
+      <c r="S16" t="s">
         <v>289</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>98</v>
-      </c>
-      <c r="S16" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="17" spans="1:19">
       <c r="F17" t="s">
+        <v>290</v>
+      </c>
+      <c r="O17" t="s">
         <v>291</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>292</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="O18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:19">
       <c r="F20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:19">
       <c r="A27" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:19">
       <c r="D31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E31" t="s">
         <v>6</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:19">
       <c r="A32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J32" t="s">
         <v>24</v>
       </c>
       <c r="R32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="2:19">
       <c r="B33" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K33" t="s">
         <v>51</v>
       </c>
       <c r="R33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="S33">
         <v>0</v>
@@ -2993,13 +2990,13 @@
     </row>
     <row r="34" spans="2:19">
       <c r="C34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K34" t="s">
         <v>54</v>
       </c>
       <c r="R34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="S34">
         <v>0.5</v>
@@ -3007,19 +3004,19 @@
     </row>
     <row r="35" spans="2:19">
       <c r="C35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="L35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="R35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S35">
         <v>1</v>
@@ -3027,13 +3024,13 @@
     </row>
     <row r="36" spans="2:19">
       <c r="D36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="L36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="R36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="S36">
         <v>1</v>
@@ -3049,10 +3046,10 @@
     </row>
     <row r="38" spans="2:19">
       <c r="C38" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K38" t="s">
         <v>2</v>
@@ -3060,13 +3057,13 @@
     </row>
     <row r="39" spans="2:19">
       <c r="C39" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E39" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="2:19">
@@ -3086,29 +3083,29 @@
     </row>
     <row r="52" spans="1:12">
       <c r="H52" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I53" s="1" t="s">
         <v>303</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="H53" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="I53" s="1" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="E54" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F54">
         <v>4</v>
@@ -3142,76 +3139,76 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="F59" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="E61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="E62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="B65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="B68" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B70">
         <v>250</v>
       </c>
       <c r="C70" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B71">
         <v>12.5</v>
       </c>
       <c r="C71" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -3243,48 +3240,48 @@
   <sheetData>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="B4" t="s">
+        <v>321</v>
+      </c>
+      <c r="I4" t="s">
+        <v>319</v>
+      </c>
+      <c r="J4" t="s">
+        <v>320</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>322</v>
       </c>
-      <c r="I4" t="s">
-        <v>320</v>
-      </c>
-      <c r="J4" t="s">
-        <v>321</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" t="s">
         <v>323</v>
       </c>
-      <c r="R4" t="s">
-        <v>324</v>
-      </c>
       <c r="S4" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="B5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I5" s="3">
         <v>14</v>
@@ -3294,18 +3291,18 @@
       </c>
       <c r="P5" s="1"/>
       <c r="Q5" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="R5" s="41" t="s">
         <v>326</v>
       </c>
-      <c r="R5" s="41" t="s">
+      <c r="S5" t="s">
         <v>327</v>
-      </c>
-      <c r="S5" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="6" spans="1:19">
       <c r="H6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I6">
         <f>I5/4</f>
@@ -3317,51 +3314,51 @@
       </c>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="R6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="R7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="H8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I8" s="5">
         <v>320</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="R8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="S8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I9" s="5">
         <v>100</v>
@@ -3369,7 +3366,7 @@
     </row>
     <row r="10" spans="1:19">
       <c r="H10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I10" s="5">
         <v>10</v>
@@ -3377,12 +3374,12 @@
     </row>
     <row r="11" spans="1:19">
       <c r="B11" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:19">
       <c r="B12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I12" s="9">
         <v>3.7</v>
@@ -3394,20 +3391,20 @@
     </row>
     <row r="16" spans="1:19">
       <c r="J16" t="s">
+        <v>334</v>
+      </c>
+      <c r="M16" t="s">
         <v>335</v>
-      </c>
-      <c r="M16" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="19" spans="10:10">
       <c r="J19" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="1048576" spans="15:15">
       <c r="O1048576" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
   </sheetData>
@@ -3686,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AW78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD37" sqref="AD37"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -4101,7 +4098,7 @@
         <v>62.499999999999964</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J5" s="15">
         <v>1</v>
@@ -4135,7 +4132,7 @@
         <v>1</v>
       </c>
       <c r="U5" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V5" s="45">
         <v>0.8</v>
@@ -4147,13 +4144,13 @@
         <v>51</v>
       </c>
       <c r="Y5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z5" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z5" s="15" t="s">
+      <c r="AA5" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="AA5" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="AB5" s="41">
         <v>20</v>
@@ -4162,16 +4159,16 @@
         <v>5</v>
       </c>
       <c r="AD5" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE5" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AE5" s="15" t="s">
+      <c r="AF5" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF5" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG5" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH5" s="18" t="b">
         <v>1</v>
@@ -4185,7 +4182,7 @@
       </c>
       <c r="AN5" s="90"/>
       <c r="AO5" s="116" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP5" s="18"/>
       <c r="AQ5" s="18" t="b">
@@ -4257,7 +4254,7 @@
       </c>
       <c r="AN6" s="90"/>
       <c r="AO6" s="116" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP6" s="18"/>
       <c r="AQ6" s="18"/>
@@ -4277,7 +4274,7 @@
         <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7">
         <v>4</v>
@@ -4347,7 +4344,7 @@
       <c r="S8" s="15"/>
       <c r="T8" s="97"/>
       <c r="U8" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="V8" s="42">
         <v>0.9</v>
@@ -4359,13 +4356,13 @@
         <v>2</v>
       </c>
       <c r="Y8" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z8" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="Z8" s="15" t="s">
+      <c r="AA8" s="15" t="s">
         <v>92</v>
-      </c>
-      <c r="AA8" s="15" t="s">
-        <v>93</v>
       </c>
       <c r="AB8" s="15"/>
       <c r="AC8" s="15"/>
@@ -4391,7 +4388,7 @@
         <v>50</v>
       </c>
       <c r="AO8" s="118" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP8" s="16" t="b">
         <v>0</v>
@@ -4403,13 +4400,13 @@
         <v>0</v>
       </c>
       <c r="AS8" s="91" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT8" s="93">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="18" t="s">
         <v>94</v>
-      </c>
-      <c r="AT8" s="93">
-        <v>0</v>
-      </c>
-      <c r="AU8" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="AV8" s="18" t="s">
         <v>2</v>
@@ -4462,7 +4459,7 @@
         <v>50</v>
       </c>
       <c r="AO9" s="118" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP9" s="16"/>
       <c r="AQ9" s="16"/>
@@ -4546,7 +4543,7 @@
       <c r="S11" s="15"/>
       <c r="T11" s="97"/>
       <c r="U11" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V11" s="15">
         <v>1</v>
@@ -4558,13 +4555,13 @@
         <v>2</v>
       </c>
       <c r="Y11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z11" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA11" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z11" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA11" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB11" s="15"/>
       <c r="AC11" s="15"/>
@@ -4602,13 +4599,13 @@
         <v>0</v>
       </c>
       <c r="AS11" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT11" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU11" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT11" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU11" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV11" s="15" t="s">
         <v>2</v>
@@ -4690,7 +4687,7 @@
       <c r="S13" s="15"/>
       <c r="T13" s="97"/>
       <c r="U13" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V13" s="15">
         <v>1</v>
@@ -4702,13 +4699,13 @@
         <v>2</v>
       </c>
       <c r="Y13" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z13" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA13" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z13" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA13" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB13" s="15"/>
       <c r="AC13" s="15"/>
@@ -4723,12 +4720,8 @@
       </c>
       <c r="AK13" s="16"/>
       <c r="AL13" s="110"/>
-      <c r="AM13" s="82" t="s">
-        <v>37</v>
-      </c>
-      <c r="AN13" s="80">
-        <v>0.5</v>
-      </c>
+      <c r="AM13" s="82"/>
+      <c r="AN13" s="80"/>
       <c r="AO13" s="119"/>
       <c r="AP13" s="16" t="b">
         <v>0</v>
@@ -4740,13 +4733,13 @@
         <v>0</v>
       </c>
       <c r="AS13" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT13" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU13" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT13" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU13" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV13" s="15" t="s">
         <v>2</v>
@@ -4816,7 +4809,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
       <c r="I15" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J15" s="15">
         <v>0</v>
@@ -4850,7 +4843,7 @@
         <v>1</v>
       </c>
       <c r="U15" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V15" s="45">
         <v>0.8</v>
@@ -4862,10 +4855,10 @@
         <v>51</v>
       </c>
       <c r="Y15" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z15" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="Z15" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="AA15" s="15"/>
       <c r="AB15" s="15">
@@ -4875,16 +4868,16 @@
         <v>5</v>
       </c>
       <c r="AD15" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE15" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AE15" s="15" t="s">
+      <c r="AF15" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF15" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG15" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH15" s="18" t="b">
         <v>1</v>
@@ -4978,7 +4971,7 @@
       <c r="S17" s="15"/>
       <c r="T17" s="97"/>
       <c r="U17" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V17" s="15">
         <v>1</v>
@@ -4990,13 +4983,13 @@
         <v>2</v>
       </c>
       <c r="Y17" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z17" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA17" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z17" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA17" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB17" s="15"/>
       <c r="AC17" s="15"/>
@@ -5034,13 +5027,13 @@
         <v>0</v>
       </c>
       <c r="AS17" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT17" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU17" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT17" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU17" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV17" s="15" t="s">
         <v>2</v>
@@ -5156,7 +5149,7 @@
       <c r="G21" s="15"/>
       <c r="H21" s="15"/>
       <c r="U21" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V21" s="15">
         <v>1</v>
@@ -5168,13 +5161,13 @@
         <v>2</v>
       </c>
       <c r="Y21" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z21" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA21" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA21" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB21" s="15"/>
       <c r="AC21" s="15"/>
@@ -5202,13 +5195,13 @@
         <v>0</v>
       </c>
       <c r="AS21" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT21" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU21" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT21" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU21" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV21" s="15" t="s">
         <v>2</v>
@@ -5278,7 +5271,7 @@
       <c r="G23" s="15"/>
       <c r="H23" s="15"/>
       <c r="I23" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J23" s="15">
         <v>0</v>
@@ -5312,7 +5305,7 @@
         <v>1</v>
       </c>
       <c r="U23" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V23" s="45">
         <v>0.8</v>
@@ -5324,13 +5317,13 @@
         <v>51</v>
       </c>
       <c r="Y23" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z23" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z23" s="15" t="s">
+      <c r="AA23" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="AA23" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="AB23" s="15">
         <v>20</v>
@@ -5339,16 +5332,16 @@
         <v>5</v>
       </c>
       <c r="AD23" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE23" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AE23" s="15" t="s">
+      <c r="AF23" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF23" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG23" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH23" s="18" t="b">
         <v>1</v>
@@ -5442,7 +5435,7 @@
       <c r="S25" s="15"/>
       <c r="T25" s="97"/>
       <c r="U25" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="V25" s="45">
         <v>0.9</v>
@@ -5454,13 +5447,13 @@
         <v>2</v>
       </c>
       <c r="Y25" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z25" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="Z25" s="15" t="s">
-        <v>92</v>
-      </c>
       <c r="AA25" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB25" s="15"/>
       <c r="AC25" s="15"/>
@@ -5486,7 +5479,7 @@
         <v>50</v>
       </c>
       <c r="AO25" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP25" s="16" t="b">
         <v>0</v>
@@ -5548,7 +5541,7 @@
         <v>50</v>
       </c>
       <c r="AO26" s="123" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP26" s="16"/>
       <c r="AQ26" s="16"/>
@@ -5630,7 +5623,7 @@
       <c r="S28" s="15"/>
       <c r="T28" s="97"/>
       <c r="U28" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V28" s="15">
         <v>1</v>
@@ -5642,13 +5635,13 @@
         <v>2</v>
       </c>
       <c r="Y28" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z28" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA28" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z28" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA28" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB28" s="15"/>
       <c r="AC28" s="15"/>
@@ -5686,13 +5679,13 @@
         <v>0</v>
       </c>
       <c r="AS28" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT28" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU28" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT28" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU28" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV28" s="15" t="s">
         <v>2</v>
@@ -5808,7 +5801,7 @@
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="U32" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V32" s="15">
         <v>1</v>
@@ -5820,13 +5813,13 @@
         <v>2</v>
       </c>
       <c r="Y32" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z32" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA32" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z32" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA32" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB32" s="15"/>
       <c r="AC32" s="15"/>
@@ -5854,13 +5847,13 @@
         <v>0</v>
       </c>
       <c r="AS32" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT32" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU32" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT32" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU32" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV32" s="15" t="s">
         <v>2</v>
@@ -5930,13 +5923,13 @@
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="J34" s="15">
+        <v>0</v>
+      </c>
+      <c r="K34" s="41" t="s">
         <v>103</v>
-      </c>
-      <c r="J34" s="15">
-        <v>0</v>
-      </c>
-      <c r="K34" s="41" t="s">
-        <v>104</v>
       </c>
       <c r="L34" s="41">
         <v>0</v>
@@ -5958,7 +5951,7 @@
       <c r="S34" s="41"/>
       <c r="T34" s="99"/>
       <c r="U34" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V34" s="15">
         <v>1</v>
@@ -5970,13 +5963,13 @@
         <v>51</v>
       </c>
       <c r="Y34" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z34" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z34" s="15" t="s">
+      <c r="AA34" s="15" t="s">
         <v>83</v>
-      </c>
-      <c r="AA34" s="15" t="s">
-        <v>84</v>
       </c>
       <c r="AB34" s="15">
         <v>20</v>
@@ -5985,7 +5978,7 @@
         <v>5</v>
       </c>
       <c r="AD34" s="97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE34" s="15"/>
       <c r="AF34" s="15"/>
@@ -6084,7 +6077,7 @@
       <c r="S36" s="15"/>
       <c r="T36" s="97"/>
       <c r="U36" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V36" s="15">
         <v>0.99</v>
@@ -6096,10 +6089,10 @@
         <v>51</v>
       </c>
       <c r="Y36" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z36" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="Z36" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="AA36" s="15"/>
       <c r="AB36" s="15">
@@ -6109,16 +6102,16 @@
         <v>1</v>
       </c>
       <c r="AD36" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE36" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF36" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF36" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG36" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH36" s="18" t="b">
         <v>1</v>
@@ -6196,7 +6189,7 @@
       <c r="A38" s="15"/>
       <c r="B38" s="15"/>
       <c r="U38" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V38" s="15">
         <v>1</v>
@@ -6208,13 +6201,13 @@
         <v>2</v>
       </c>
       <c r="Y38" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z38" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA38" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z38" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA38" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB38" s="15"/>
       <c r="AC38" s="15"/>
@@ -6242,13 +6235,13 @@
         <v>0</v>
       </c>
       <c r="AS38" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT38" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU38" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT38" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU38" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV38" s="15" t="s">
         <v>2</v>
@@ -6318,13 +6311,13 @@
       <c r="G40" s="15"/>
       <c r="H40" s="15"/>
       <c r="I40" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J40" s="15">
         <v>0</v>
       </c>
       <c r="K40" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L40" s="41">
         <v>0</v>
@@ -6346,7 +6339,7 @@
       <c r="S40" s="15"/>
       <c r="T40" s="97"/>
       <c r="U40" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V40" s="15">
         <v>1</v>
@@ -6358,14 +6351,14 @@
         <v>51</v>
       </c>
       <c r="Y40" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z40" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z40" s="15" t="s">
+      <c r="AA40" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="AA40" s="15" t="s">
-        <v>84</v>
-      </c>
       <c r="AB40" s="15">
         <v>0</v>
       </c>
@@ -6373,7 +6366,7 @@
         <v>1</v>
       </c>
       <c r="AD40" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE40" s="15"/>
       <c r="AF40" s="15"/>
@@ -6436,7 +6429,7 @@
       <c r="A42" s="15"/>
       <c r="B42" s="15"/>
       <c r="U42" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V42" s="15">
         <v>1</v>
@@ -6448,13 +6441,13 @@
         <v>2</v>
       </c>
       <c r="Y42" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z42" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA42" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z42" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA42" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB42" s="15"/>
       <c r="AC42" s="15"/>
@@ -6482,13 +6475,13 @@
         <v>0</v>
       </c>
       <c r="AS42" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT42" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU42" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT42" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU42" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV42" s="15" t="s">
         <v>2</v>
@@ -6558,13 +6551,13 @@
       <c r="G44" s="15"/>
       <c r="H44" s="15"/>
       <c r="I44" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J44" s="15">
         <v>0</v>
       </c>
       <c r="K44" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L44" s="41">
         <v>0</v>
@@ -6586,7 +6579,7 @@
       <c r="S44" s="15"/>
       <c r="T44" s="97"/>
       <c r="U44" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="V44" s="15">
         <v>1</v>
@@ -6598,14 +6591,14 @@
         <v>51</v>
       </c>
       <c r="Y44" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z44" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z44" s="15" t="s">
+      <c r="AA44" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="AA44" s="15" t="s">
-        <v>84</v>
-      </c>
       <c r="AB44" s="15">
         <v>0</v>
       </c>
@@ -6613,7 +6606,7 @@
         <v>1</v>
       </c>
       <c r="AD44" s="97" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE44" s="15"/>
       <c r="AF44" s="15"/>
@@ -6694,7 +6687,7 @@
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="U46" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V46" s="15">
         <v>1</v>
@@ -6706,13 +6699,13 @@
         <v>2</v>
       </c>
       <c r="Y46" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z46" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA46" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z46" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA46" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB46" s="15"/>
       <c r="AC46" s="15"/>
@@ -6740,13 +6733,13 @@
         <v>0</v>
       </c>
       <c r="AS46" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT46" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU46" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT46" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU46" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV46" s="15" t="s">
         <v>2</v>
@@ -6816,7 +6809,7 @@
       <c r="G48" s="15"/>
       <c r="H48" s="15"/>
       <c r="I48" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J48" s="15">
         <v>0</v>
@@ -6852,7 +6845,7 @@
         <v>2</v>
       </c>
       <c r="U48" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V48" s="15">
         <v>1</v>
@@ -6864,16 +6857,16 @@
         <v>51</v>
       </c>
       <c r="Y48" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z48" s="15" t="s">
         <v>82</v>
-      </c>
-      <c r="Z48" s="15" t="s">
-        <v>83</v>
       </c>
       <c r="AA48" s="15"/>
       <c r="AB48" s="15"/>
       <c r="AC48" s="15"/>
       <c r="AD48" s="97" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AE48" s="15"/>
       <c r="AF48" s="15"/>
@@ -6986,7 +6979,7 @@
       <c r="S50" s="15"/>
       <c r="T50" s="97"/>
       <c r="U50" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="V50" s="15">
         <v>1</v>
@@ -6998,13 +6991,13 @@
         <v>2</v>
       </c>
       <c r="Y50" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z50" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA50" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z50" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA50" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB50" s="15"/>
       <c r="AC50" s="15"/>
@@ -7042,13 +7035,13 @@
         <v>0</v>
       </c>
       <c r="AS50" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT50" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU50" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT50" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU50" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV50" s="15" t="s">
         <v>2</v>
@@ -7164,7 +7157,7 @@
       <c r="A54" s="15"/>
       <c r="B54" s="15"/>
       <c r="U54" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="V54" s="15">
         <v>1</v>
@@ -7176,13 +7169,13 @@
         <v>2</v>
       </c>
       <c r="Y54" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z54" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA54" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z54" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA54" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB54" s="15"/>
       <c r="AC54" s="15"/>
@@ -7210,13 +7203,13 @@
         <v>0</v>
       </c>
       <c r="AS54" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT54" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU54" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT54" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU54" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV54" s="15" t="s">
         <v>2</v>
@@ -7281,20 +7274,20 @@
       <c r="B56" s="15"/>
       <c r="C56" s="41"/>
       <c r="D56" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="E56" t="s">
         <v>110</v>
       </c>
-      <c r="E56" t="s">
-        <v>111</v>
-      </c>
       <c r="F56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G56" s="15" t="b">
         <v>0</v>
       </c>
       <c r="H56" s="15"/>
       <c r="I56" s="42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J56" s="42">
         <v>0</v>
@@ -7318,13 +7311,13 @@
         <v>10</v>
       </c>
       <c r="Q56" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="R56" s="15"/>
       <c r="S56" s="15"/>
       <c r="T56" s="97"/>
       <c r="U56" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V56" s="15">
         <v>0.8</v>
@@ -7336,13 +7329,13 @@
         <v>51</v>
       </c>
       <c r="Y56" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z56" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z56" s="15" t="s">
+      <c r="AA56" s="41" t="s">
         <v>83</v>
-      </c>
-      <c r="AA56" s="41" t="s">
-        <v>84</v>
       </c>
       <c r="AB56" s="15">
         <v>20</v>
@@ -7351,16 +7344,16 @@
         <v>5</v>
       </c>
       <c r="AD56" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE56" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AE56" s="15" t="s">
+      <c r="AF56" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF56" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG56" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH56" s="18" t="b">
         <v>1</v>
@@ -7456,7 +7449,7 @@
       <c r="S58" s="15"/>
       <c r="T58" s="97"/>
       <c r="U58" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="V58" s="15">
         <v>1</v>
@@ -7468,13 +7461,13 @@
         <v>2</v>
       </c>
       <c r="Y58" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z58" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA58" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z58" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA58" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB58" s="15"/>
       <c r="AC58" s="15"/>
@@ -7512,13 +7505,13 @@
         <v>0</v>
       </c>
       <c r="AS58" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT58" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU58" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT58" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU58" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV58" s="15" t="s">
         <v>2</v>
@@ -7671,7 +7664,7 @@
       <c r="S62" s="15"/>
       <c r="T62" s="97"/>
       <c r="U62" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="V62" s="15">
         <v>1</v>
@@ -7683,13 +7676,13 @@
         <v>69</v>
       </c>
       <c r="Y62" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z62" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA62" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z62" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA62" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB62" s="15"/>
       <c r="AC62" s="15"/>
@@ -7717,13 +7710,13 @@
         <v>0</v>
       </c>
       <c r="AS62" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT62" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU62" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT62" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU62" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV62" s="15" t="s">
         <v>2</v>
@@ -7788,20 +7781,20 @@
       <c r="B64" s="15"/>
       <c r="C64" s="41"/>
       <c r="D64" s="99" t="s">
+        <v>115</v>
+      </c>
+      <c r="E64" t="s">
         <v>116</v>
       </c>
-      <c r="E64" t="s">
-        <v>117</v>
-      </c>
       <c r="F64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G64" s="15" t="b">
         <v>0</v>
       </c>
       <c r="H64" s="15"/>
       <c r="I64" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J64" s="15">
         <v>0</v>
@@ -7831,7 +7824,7 @@
       <c r="S64" s="15"/>
       <c r="T64" s="97"/>
       <c r="U64" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="V64" s="15">
         <v>0.8</v>
@@ -7843,13 +7836,13 @@
         <v>51</v>
       </c>
       <c r="Y64" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z64" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="Z64" s="15" t="s">
+      <c r="AA64" s="41" t="s">
         <v>83</v>
-      </c>
-      <c r="AA64" s="41" t="s">
-        <v>84</v>
       </c>
       <c r="AB64" s="15">
         <v>20</v>
@@ -7858,16 +7851,16 @@
         <v>5</v>
       </c>
       <c r="AD64" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE64" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="AE64" s="15" t="s">
+      <c r="AF64" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="AF64" s="15" t="s">
-        <v>87</v>
-      </c>
       <c r="AG64" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AH64" s="18" t="b">
         <v>1</v>
@@ -7965,7 +7958,7 @@
       <c r="S66" s="15"/>
       <c r="T66" s="97"/>
       <c r="U66" s="45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="V66" s="15">
         <v>1</v>
@@ -7977,13 +7970,13 @@
         <v>2</v>
       </c>
       <c r="Y66" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z66" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA66" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z66" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA66" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB66" s="15"/>
       <c r="AC66" s="15"/>
@@ -8021,13 +8014,13 @@
         <v>0</v>
       </c>
       <c r="AS66" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT66" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU66" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT66" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU66" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV66" s="15" t="s">
         <v>2</v>
@@ -8180,7 +8173,7 @@
       <c r="S70" s="15"/>
       <c r="T70" s="97"/>
       <c r="U70" s="45" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V70" s="15">
         <v>1</v>
@@ -8192,13 +8185,13 @@
         <v>69</v>
       </c>
       <c r="Y70" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z70" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="AA70" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="Z70" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="AA70" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="AB70" s="15"/>
       <c r="AC70" s="15"/>
@@ -8226,13 +8219,13 @@
         <v>0</v>
       </c>
       <c r="AS70" s="76" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT70" s="19">
+        <v>1</v>
+      </c>
+      <c r="AU70" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AT70" s="19">
-        <v>1</v>
-      </c>
-      <c r="AU70" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AV70" s="15" t="s">
         <v>2</v>
@@ -8297,16 +8290,16 @@
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="97" t="s">
+        <v>119</v>
+      </c>
+      <c r="E72" s="15" t="s">
         <v>120</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>121</v>
       </c>
       <c r="F72" s="15"/>
       <c r="G72" s="15"/>
       <c r="H72" s="15"/>
       <c r="I72" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="J72" s="15">
         <v>0</v>
@@ -8330,13 +8323,13 @@
         <v>10</v>
       </c>
       <c r="Q72" s="15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="R72" s="15"/>
       <c r="S72" s="15"/>
       <c r="T72" s="97"/>
       <c r="U72" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V72" s="15">
         <v>0.9</v>
@@ -8348,25 +8341,25 @@
         <v>2</v>
       </c>
       <c r="Y72" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Z72" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AA72" s="15"/>
       <c r="AB72" s="15"/>
       <c r="AC72" s="15"/>
       <c r="AD72" s="97" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AE72" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AF72" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AG72" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="AH72" s="16" t="b">
         <v>1</v>
@@ -8388,7 +8381,7 @@
         <v>50</v>
       </c>
       <c r="AO72" s="120" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP72" s="16"/>
       <c r="AQ72" s="16"/>
@@ -8400,7 +8393,7 @@
         <v>50</v>
       </c>
       <c r="AU72" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AV72" s="15"/>
       <c r="AW72" s="15" t="s">
@@ -8413,7 +8406,7 @@
       <c r="C73" s="15"/>
       <c r="D73" s="97"/>
       <c r="E73" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F73" s="15"/>
       <c r="G73" s="15"/>
@@ -8455,7 +8448,7 @@
         <v>170</v>
       </c>
       <c r="AO73" s="120" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AP73" s="16"/>
       <c r="AQ73" s="16"/>
@@ -8467,7 +8460,7 @@
         <v>50</v>
       </c>
       <c r="AU73" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AV73" s="15"/>
       <c r="AW73" s="15"/>
@@ -8931,39 +8924,39 @@
     <row r="2" spans="1:20">
       <c r="J2" s="1"/>
       <c r="Q2" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="R2" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="27" t="s">
+      <c r="S2" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="S2" s="27" t="s">
+      <c r="T2" s="27" t="s">
         <v>130</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" t="s">
         <v>132</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>133</v>
-      </c>
-      <c r="D3" t="s">
-        <v>134</v>
       </c>
       <c r="Q3" s="28"/>
     </row>
     <row r="4" spans="1:20">
       <c r="B4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="R4" s="29"/>
       <c r="S4" s="29"/>
@@ -8971,7 +8964,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="B5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Q5" s="29"/>
       <c r="R5" s="30" t="s">
@@ -8982,7 +8975,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="B6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="Q6" s="31"/>
       <c r="R6" s="31"/>
@@ -8993,72 +8986,72 @@
     </row>
     <row r="7" spans="1:20">
       <c r="B7" t="s">
+        <v>137</v>
+      </c>
+      <c r="T7" t="s">
         <v>138</v>
-      </c>
-      <c r="T7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="T8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:20">
       <c r="T9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="T10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="T11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:20">
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="T12" s="31"/>
     </row>
     <row r="13" spans="1:20">
       <c r="T13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:20">
       <c r="Q14" s="31"/>
       <c r="R14" s="31"/>
       <c r="S14" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="T14" s="31"/>
     </row>
     <row r="15" spans="1:20">
       <c r="T15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="T16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="17:20">
       <c r="T17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="17:20">
       <c r="Q18" s="29"/>
       <c r="R18" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
@@ -9067,85 +9060,85 @@
       <c r="Q19" s="31"/>
       <c r="R19" s="31"/>
       <c r="S19" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="T19" s="31"/>
     </row>
     <row r="20" spans="17:20">
       <c r="T20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="17:20">
       <c r="Q21" s="28"/>
       <c r="S21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="17:20">
       <c r="Q22" s="28"/>
       <c r="T22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="17:20">
       <c r="Q23" s="28"/>
       <c r="S23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="17:20">
       <c r="Q24" s="28"/>
       <c r="T24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="17:20">
       <c r="Q25" s="28"/>
       <c r="T25" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="17:20">
       <c r="Q26" s="28"/>
       <c r="S26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="17:20">
       <c r="Q27" s="28"/>
       <c r="S27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="17:20">
       <c r="Q28" s="28"/>
       <c r="T28" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="17:20">
       <c r="Q29" s="28"/>
       <c r="S29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="17:20">
       <c r="Q30" s="28"/>
       <c r="T30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="17:20">
       <c r="Q31" s="28"/>
       <c r="T31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="17:20">
       <c r="Q32" s="29"/>
       <c r="R32" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
@@ -9154,34 +9147,34 @@
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="T33" s="31"/>
     </row>
     <row r="34" spans="17:20">
       <c r="Q34" s="28"/>
       <c r="T34" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="35" spans="17:20">
       <c r="Q35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="T35" s="31"/>
     </row>
     <row r="36" spans="17:20">
       <c r="Q36" s="28"/>
       <c r="T36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="17:20">
       <c r="Q37" s="29"/>
       <c r="R37" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
@@ -9190,28 +9183,28 @@
       <c r="Q38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T38" s="31"/>
     </row>
     <row r="39" spans="17:20">
       <c r="Q39" s="28"/>
       <c r="T39" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="17:20">
       <c r="Q40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="T40" s="31"/>
     </row>
     <row r="41" spans="17:20">
       <c r="Q41" s="28"/>
       <c r="T41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -9252,7 +9245,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
       <c r="H1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -9278,12 +9271,12 @@
         <v>15</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B3">
         <v>50</v>
@@ -9323,24 +9316,24 @@
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>170</v>
-      </c>
-      <c r="E5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -9352,18 +9345,18 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H7" t="s">
         <v>38</v>
@@ -9371,7 +9364,7 @@
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B8">
         <v>80</v>
@@ -9397,7 +9390,7 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
         <v>79</v>
@@ -9408,7 +9401,7 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E10" t="s">
         <v>79</v>
@@ -9419,7 +9412,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B11" s="42"/>
       <c r="C11" s="42"/>
@@ -9427,7 +9420,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -9448,13 +9441,13 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J12" s="45"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F13">
         <v>25</v>
@@ -9462,22 +9455,22 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -9489,15 +9482,15 @@
         <v>10</v>
       </c>
       <c r="E19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B20">
         <v>50</v>
@@ -9509,10 +9502,10 @@
         <v>10</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -9538,10 +9531,10 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -9555,7 +9548,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
@@ -9580,10 +9573,10 @@
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5" t="s">
         <v>186</v>
-      </c>
-      <c r="C5" t="s">
-        <v>187</v>
       </c>
       <c r="D5">
         <v>4</v>
@@ -9592,53 +9585,53 @@
         <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" t="s">
         <v>189</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>190</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="B10" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3">
@@ -9701,7 +9694,7 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R1" s="22"/>
       <c r="S1" s="22"/>
@@ -9713,7 +9706,7 @@
       <c r="Y1" s="24"/>
       <c r="Z1" s="52"/>
       <c r="AA1" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AB1" s="21"/>
       <c r="AC1" s="21"/>
@@ -9726,7 +9719,7 @@
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1">
       <c r="C2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2" s="25"/>
       <c r="F2" s="25"/>
@@ -9767,7 +9760,7 @@
       <c r="AC2" s="21"/>
       <c r="AD2" s="49"/>
       <c r="AE2" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AF2" s="4"/>
       <c r="AG2" s="4"/>
@@ -9782,7 +9775,7 @@
         <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>58</v>
@@ -9806,7 +9799,7 @@
         <v>63</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>64</v>
@@ -9837,7 +9830,7 @@
       </c>
       <c r="V3" s="55"/>
       <c r="W3" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X3" s="24" t="s">
         <v>26</v>
@@ -9857,7 +9850,7 @@
       </c>
       <c r="AD3" s="49"/>
       <c r="AE3" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AF3" s="4" t="s">
         <v>75</v>
@@ -9875,10 +9868,10 @@
         <v>28</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E4" s="15">
         <v>0.8</v>
@@ -9890,10 +9883,10 @@
         <v>51</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J4" s="15">
         <v>20</v>
@@ -9902,28 +9895,28 @@
         <v>5</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M4" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q4" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="N4" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="O4" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="P4" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q4" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="18" t="s">
-        <v>203</v>
-      </c>
       <c r="S4" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
@@ -9965,7 +9958,7 @@
     </row>
     <row r="6" spans="1:35" s="15" customFormat="1">
       <c r="C6" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E6" s="15">
         <v>0.9</v>
@@ -9977,13 +9970,13 @@
         <v>69</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="Q6" s="16" t="b">
         <v>1</v>
@@ -10004,7 +9997,7 @@
         <v>50</v>
       </c>
       <c r="Y6" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z6" s="53"/>
       <c r="AA6" s="16" t="b">
@@ -10037,7 +10030,7 @@
         <v>50</v>
       </c>
       <c r="Y7" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z7" s="53"/>
       <c r="AA7" s="16" t="b">
@@ -10071,7 +10064,7 @@
     </row>
     <row r="9" spans="1:35" s="15" customFormat="1">
       <c r="C9" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E9" s="15">
         <v>1</v>
@@ -10083,10 +10076,10 @@
         <v>69</v>
       </c>
       <c r="H9" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="I9" s="15" t="s">
         <v>97</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>98</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>6</v>
@@ -10124,13 +10117,13 @@
       </c>
       <c r="AD9" s="50"/>
       <c r="AE9" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AF9" s="15">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="15" t="s">
         <v>94</v>
-      </c>
-      <c r="AF9" s="15">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="15" t="s">
-        <v>95</v>
       </c>
       <c r="AH9" s="15" t="s">
         <v>2</v>
@@ -10218,10 +10211,10 @@
         <v>28</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E15" s="15">
         <v>0.8</v>
@@ -10230,10 +10223,10 @@
         <v>50</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J15" s="15">
         <v>20</v>
@@ -10242,66 +10235,66 @@
         <v>5</v>
       </c>
       <c r="M15" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="O15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="P15" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q15" s="18" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="N15" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="P15" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q15" s="18" t="b">
-        <v>1</v>
-      </c>
-      <c r="R15" s="18" t="s">
-        <v>203</v>
-      </c>
       <c r="S15" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T15" s="18"/>
       <c r="U15" s="18"/>
       <c r="V15" s="50"/>
       <c r="W15" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="X15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Y15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z15" s="50"/>
       <c r="AA15" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AD15" s="50"/>
       <c r="AE15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AF15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AG15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AH15" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AI15" s="47"/>
     </row>
     <row r="16" spans="1:35" s="15" customFormat="1">
       <c r="C16" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" s="15">
         <v>0.9</v>
@@ -10313,7 +10306,7 @@
         <v>54</v>
       </c>
       <c r="H16" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q16" s="16" t="b">
         <v>1</v>
@@ -10334,7 +10327,7 @@
         <v>50</v>
       </c>
       <c r="Y16" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z16" s="53"/>
       <c r="AA16" s="16" t="b">
@@ -10348,16 +10341,16 @@
       </c>
       <c r="AD16" s="50"/>
       <c r="AE16" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AF16" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AG16" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AH16" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AI16" s="47"/>
     </row>
@@ -10375,7 +10368,7 @@
         <v>50</v>
       </c>
       <c r="Y17" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z17" s="53"/>
       <c r="AA17" s="16" t="b">
@@ -10392,7 +10385,7 @@
     </row>
     <row r="18" spans="1:35" s="15" customFormat="1">
       <c r="C18" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E18" s="15">
         <v>1</v>
@@ -10404,7 +10397,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q18" s="16" t="b">
         <v>1</v>
@@ -10504,7 +10497,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E21" s="15">
         <v>1</v>
@@ -10516,36 +10509,36 @@
         <v>2</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q21" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="R21" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S21" s="15" t="b">
         <v>1</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="X21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Y21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Z21" s="47"/>
       <c r="AA21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AD21" s="47"/>
       <c r="AE21"/>
@@ -10572,7 +10565,7 @@
     </row>
     <row r="23" spans="1:35" s="15" customFormat="1">
       <c r="C23" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E23" s="15">
         <v>0.9</v>
@@ -10584,22 +10577,22 @@
         <v>2</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L23" s="15" t="s">
         <v>6</v>
       </c>
       <c r="M23" s="15" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="N23" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="O23" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P23" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q23" s="16" t="b">
         <v>1</v>
@@ -10622,17 +10615,17 @@
         <v>50</v>
       </c>
       <c r="Y23" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z23" s="53"/>
       <c r="AA23" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB23" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC23" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AD23" s="50"/>
       <c r="AE23" s="16" t="s">
@@ -10642,7 +10635,7 @@
         <v>50</v>
       </c>
       <c r="AG23" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI23" s="47"/>
     </row>
@@ -10660,17 +10653,17 @@
         <v>170</v>
       </c>
       <c r="Y24" s="19" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Z24" s="53"/>
       <c r="AA24" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AB24" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AC24" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="AD24" s="50"/>
       <c r="AE24" s="16" t="s">
@@ -10680,7 +10673,7 @@
         <v>50</v>
       </c>
       <c r="AG24" s="16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI24" s="47"/>
     </row>
@@ -10825,19 +10818,19 @@
   <sheetData>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>59</v>
@@ -10851,19 +10844,19 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -10871,18 +10864,18 @@
     </row>
     <row r="4" spans="1:8">
       <c r="C4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="C5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -10894,7 +10887,7 @@
         <v>100000</v>
       </c>
       <c r="G5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -10936,7 +10929,7 @@
         <v>208</v>
       </c>
       <c r="E9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9">
         <v>3500</v>
@@ -10944,19 +10937,19 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>59</v>
@@ -10964,36 +10957,36 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13">
         <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14">
         <v>36</v>
@@ -11001,7 +10994,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="C15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -11015,13 +11008,13 @@
     </row>
     <row r="16" spans="1:8">
       <c r="C16" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16">
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F16">
         <v>7000</v>
@@ -11069,226 +11062,226 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>218</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>219</v>
       </c>
       <c r="C4" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="33" t="s">
         <v>218</v>
-      </c>
-      <c r="B5" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="C5" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="32" t="s">
         <v>218</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>219</v>
       </c>
       <c r="C6" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="33" t="s">
         <v>218</v>
-      </c>
-      <c r="B7" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="C7" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D7" s="33" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="32" t="s">
         <v>218</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>219</v>
       </c>
       <c r="C8" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D8" s="32" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="33" t="s">
         <v>218</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>219</v>
       </c>
       <c r="C9" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D9" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B10" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C10" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B11" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B11" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C11" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C12" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B13" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C13" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B14" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C14" s="34" t="e">
         <v>#REF!</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="32" t="s">
+        <v>217</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>219</v>
       </c>
       <c r="C15" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D15" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C16" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D16" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" s="33" t="s">
         <v>233</v>
-      </c>
-      <c r="B17" s="33" t="s">
-        <v>234</v>
       </c>
       <c r="C17" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D17" s="33" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B18" s="32" t="s">
         <v>233</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>234</v>
       </c>
       <c r="C18" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D18" s="32" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C19" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D19" s="33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -11309,72 +11302,72 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="32" t="s">
         <v>236</v>
-      </c>
-      <c r="B22" s="32" t="s">
-        <v>237</v>
       </c>
       <c r="C22" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D22" s="32" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B23" s="33" t="s">
         <v>236</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>237</v>
       </c>
       <c r="C23" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="B24" s="32" t="s">
         <v>236</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>237</v>
       </c>
       <c r="C24" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D24" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="33" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C25" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C26" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -11387,86 +11380,86 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="B28" s="32" t="s">
         <v>243</v>
-      </c>
-      <c r="B28" s="32" t="s">
-        <v>244</v>
       </c>
       <c r="C28" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D28" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C29" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C30" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B31" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C31" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D31" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C32" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D32" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="33" t="s">
+        <v>247</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>248</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>249</v>
       </c>
       <c r="C33" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D33" s="36" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -11479,72 +11472,72 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="33" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D35" s="33" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="32" t="s">
         <v>250</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>251</v>
       </c>
       <c r="C36" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D36" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="B37" s="33" t="s">
         <v>250</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>251</v>
       </c>
       <c r="C37" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="32" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C38" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="33" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B39" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C39" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D39" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -11565,16 +11558,16 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C42" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -11587,226 +11580,226 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="32" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C44" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D44" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="33" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C45" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D45" s="33" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B46" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C46" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D46" s="32" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C47" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D47" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="32" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B48" s="39" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C48" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C49" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D49" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B50" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C50" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C51" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D51" s="33" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="32" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B52" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C52" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D52" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="33" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C53" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C54" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D54" s="32" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B55" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C55" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D55" s="33" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="32" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C56" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B57" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C57" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D57" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="32" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B58" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C58" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="33" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C59" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D59" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -11819,86 +11812,86 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="33" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B61" s="36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C61" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D61" s="33" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="32" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C62" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D62" s="32" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B63" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C63" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D63" s="33" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C64" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D64" s="32" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B65" s="33" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C65" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D65" s="33" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B66" s="32" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C66" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D66" s="32" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -11919,44 +11912,44 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="33" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B69" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C69" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D69" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="32" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C70" s="32" t="e">
         <v>#REF!</v>
       </c>
       <c r="D70" s="32" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="33" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B71" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C71" s="33" t="e">
         <v>#REF!</v>
       </c>
       <c r="D71" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to forecast table
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2234" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E6D1C31-637B-46AF-AB7E-E1D30A9F6E13}"/>
+  <xr:revisionPtr revIDLastSave="2240" documentId="11_4669E9524D91413C1C566AE84EAFB5F40377797C" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E4C9BDB1-D4A9-400D-88A6-AD9176B88779}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="337">
   <si>
     <t>Cause</t>
   </si>
@@ -3683,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AW78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="Q20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AD48" sqref="AD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1"/>
@@ -5490,10 +5490,18 @@
       <c r="AR25" s="110" t="b">
         <v>0</v>
       </c>
-      <c r="AS25" s="74"/>
-      <c r="AT25" s="93"/>
-      <c r="AU25" s="18"/>
-      <c r="AV25" s="18"/>
+      <c r="AS25" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="AT25" s="93">
+        <v>0</v>
+      </c>
+      <c r="AU25" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="AV25" s="18" t="s">
+        <v>2</v>
+      </c>
       <c r="AW25" s="15"/>
     </row>
     <row r="26" spans="1:49">
@@ -6863,8 +6871,12 @@
         <v>82</v>
       </c>
       <c r="AA48" s="15"/>
-      <c r="AB48" s="15"/>
-      <c r="AC48" s="15"/>
+      <c r="AB48" s="15">
+        <v>20</v>
+      </c>
+      <c r="AC48" s="15">
+        <v>5</v>
+      </c>
       <c r="AD48" s="97" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
disable checkboxes, unit test fix, excel update
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkirton1\OneDrive - KPMG\Documents\Essential Energy\Probability of Failure Model\inputs\model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkirton1\OneDrive - KPMG\Documents\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFC3C0A9-9142-4AE4-A768-CD34824587E3}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D28E63D-327A-402D-98CF-50A2E87A6ACD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -188,7 +188,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1052" uniqueCount="339">
   <si>
     <t>Cause</t>
   </si>
@@ -1822,7 +1822,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{FE42BDC6-EBD5-43A7-A342-17D1DCC45724}"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="103">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3320,7 +3327,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O13:O15 O17:O18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3790,8 +3797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N73" sqref="N73"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -3802,15 +3809,15 @@
     <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="13.109375" customWidth="1"/>
     <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="138" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="159" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="162" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="132" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="138" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="159" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="6" style="162" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="132" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -5832,13 +5839,13 @@
       <c r="AM28" s="16"/>
       <c r="AN28" s="110"/>
       <c r="AO28" s="84" t="s">
-        <v>32</v>
-      </c>
-      <c r="AP28" s="19">
-        <v>0</v>
-      </c>
-      <c r="AQ28" s="120">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="AP28" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="AQ28" s="122">
+        <v>3</v>
       </c>
       <c r="AR28" s="16" t="b">
         <v>0</v>
@@ -5902,15 +5909,9 @@
       <c r="AL29" s="15"/>
       <c r="AM29" s="15"/>
       <c r="AN29" s="97"/>
-      <c r="AO29" s="84" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP29" s="19">
-        <v>0</v>
-      </c>
-      <c r="AQ29" s="120">
-        <v>50</v>
-      </c>
+      <c r="AO29" s="84"/>
+      <c r="AP29" s="19"/>
+      <c r="AQ29" s="120"/>
       <c r="AR29" s="16"/>
       <c r="AS29" s="16"/>
       <c r="AT29" s="110"/>
@@ -5923,15 +5924,7 @@
     <row r="30" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
-      <c r="AO30" s="84" t="s">
-        <v>37</v>
-      </c>
-      <c r="AP30" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="AQ30" s="122">
-        <v>3</v>
-      </c>
+      <c r="AO30" s="84"/>
     </row>
     <row r="31" spans="1:51" x14ac:dyDescent="0.3">
       <c r="A31" s="15"/>
@@ -8723,191 +8716,196 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:B11 AA15 C21:D21 E20:H21 B65:B68 B14:B21 C16:D18 E15:H17 C7:G7 AG48:AR48 AO17:AT18 AR37:AT37 AR16:AY16 AR45:AY45 AR41:AY41 AR24:AY26 AR35:AT35 AU35:AY37 AO66:AY67 AR65:AY65 AO70:AY70 AR69:AY69 AO58:AY59 AR57:AY57 AO62:AY62 AR61:AY61 S35:V38 S46:V46 S69:V70 S59:V59 S32:V32 S27:V29 S74:X75 S25:AB25 B5:G6 AO36:AT36 S40:V42 B33:H54 AC15:AF15 W16:AE16 W69:AE69 W65:AE65 W35:AN35 W61:AE61 Z74:AE75 AB22:AX22 S26:AE26 AF58:AI58 S24:AN24 S57:AE58 AF57:AN57 AY57:AY58 S71:AE73 AF71:AX75 S33:AX33 S43:AX43 AF47:AX47 S39:AX39 AD34:AT34 AA17:AE17 AF16:AN17 W20:AN20 W37:AN37 S45:AN45 W41:AN41 AD23:AF23 AD25:AE25 AF25:AQ26 AR20:AY20 X66:AE66 AF65:AN66 AY64:AY66 X70:AE70 AF69:AN70 AY69:AY75 AC36:AF36 X62:AE62 AF61:AN62 AY61:AY62 C9:G11 C8:F8 W40:AB40 S47:AE48 AD40:AR40 AD44:AR44 AY22:AY26 AY33:AY37 AY39:AY41 AY43:AY45 AY47:AY48 AY15:AY17 C22:H23 B56:N56 B64:N64 AJ15:AR15 AT15:AY15 AJ23:AR23 AT23:AY23 AT40 AT44 AT48 P15:W15 P23:W23 P34:AB34 P44:AB44 P56:AY56 P64:AX64 P21:V21 I21:N29 P16:V18 I16:N18 P32:R33 I32:N54 P22:Z22 P65:V67 C65:N67 P69:R75 B69:N75 P57:R59 C57:N59 P61:V62 B61:N62 P24:R29 P35:R43 P45:R48 P49:V54 P14:Z14 C14:N15 P12:AN13 K5:N13 P7:AE11 P5:AQ6">
-    <cfRule type="cellIs" dxfId="101" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="247" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X15:Y15">
-    <cfRule type="cellIs" dxfId="100" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="245" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF15">
+    <cfRule type="cellIs" dxfId="100" priority="243" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG15:AI15">
     <cfRule type="cellIs" dxfId="99" priority="242" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG15:AI15">
+  <conditionalFormatting sqref="Z15:AB15">
     <cfRule type="cellIs" dxfId="98" priority="241" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z15:AB15">
-    <cfRule type="cellIs" dxfId="97" priority="240" operator="equal">
+  <conditionalFormatting sqref="X33:Z33">
+    <cfRule type="cellIs" dxfId="97" priority="235" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X33:Z33">
+  <conditionalFormatting sqref="X34:Y34">
     <cfRule type="cellIs" dxfId="96" priority="234" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X34:Y34">
-    <cfRule type="cellIs" dxfId="95" priority="233" operator="equal">
+  <conditionalFormatting sqref="AF34">
+    <cfRule type="cellIs" dxfId="95" priority="232" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF34">
+  <conditionalFormatting sqref="AG34:AI34">
     <cfRule type="cellIs" dxfId="94" priority="231" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG34:AI34">
+  <conditionalFormatting sqref="Z34:AB34">
     <cfRule type="cellIs" dxfId="93" priority="230" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z34:AB34">
-    <cfRule type="cellIs" dxfId="92" priority="229" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AU34:AY34">
-    <cfRule type="cellIs" dxfId="91" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="225" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU17:AY18 AO19 W17:Y17">
-    <cfRule type="cellIs" dxfId="90" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="215" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X44:Y44">
+    <cfRule type="cellIs" dxfId="90" priority="196" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF44">
     <cfRule type="cellIs" dxfId="89" priority="195" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF44">
+  <conditionalFormatting sqref="AG44:AI44">
     <cfRule type="cellIs" dxfId="88" priority="194" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG44:AI44">
+  <conditionalFormatting sqref="Z44:AB44">
     <cfRule type="cellIs" dxfId="87" priority="193" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z44:AB44">
-    <cfRule type="cellIs" dxfId="86" priority="192" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AU44:AY44">
-    <cfRule type="cellIs" dxfId="85" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="190" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X48:Y48">
-    <cfRule type="cellIs" dxfId="84" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="178" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG48:AI48">
+    <cfRule type="cellIs" dxfId="84" priority="176" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z48:AB48">
     <cfRule type="cellIs" dxfId="83" priority="175" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z48:AB48">
-    <cfRule type="cellIs" dxfId="82" priority="174" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AU48:AY48">
-    <cfRule type="cellIs" dxfId="81" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="172" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X40:Y40">
+    <cfRule type="cellIs" dxfId="81" priority="160" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF40">
     <cfRule type="cellIs" dxfId="80" priority="159" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF40">
+  <conditionalFormatting sqref="AG40:AI40">
     <cfRule type="cellIs" dxfId="79" priority="158" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG40:AI40">
+  <conditionalFormatting sqref="Z40:AB40">
     <cfRule type="cellIs" dxfId="78" priority="157" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z40:AB40">
-    <cfRule type="cellIs" dxfId="77" priority="156" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AU40:AY40">
-    <cfRule type="cellIs" dxfId="76" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="154" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA22:AA23 B22:B32 C24:D29 E24:H28 C32:D32 E31:H32">
+    <cfRule type="cellIs" dxfId="76" priority="144" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X23:Y23">
     <cfRule type="cellIs" dxfId="75" priority="143" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X23:Y23">
+  <conditionalFormatting sqref="AF23">
     <cfRule type="cellIs" dxfId="74" priority="142" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF23">
+  <conditionalFormatting sqref="AG23:AI23">
     <cfRule type="cellIs" dxfId="73" priority="141" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG23:AI23">
+  <conditionalFormatting sqref="Z23:AB23">
     <cfRule type="cellIs" dxfId="72" priority="140" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z23:AB23">
-    <cfRule type="cellIs" dxfId="71" priority="139" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AO68">
-    <cfRule type="cellIs" dxfId="70" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="120" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17">
+    <cfRule type="cellIs" dxfId="70" priority="110" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC44">
     <cfRule type="cellIs" dxfId="69" priority="109" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC44">
+  <conditionalFormatting sqref="AC40">
     <cfRule type="cellIs" dxfId="68" priority="108" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC40">
+  <conditionalFormatting sqref="AC34">
     <cfRule type="cellIs" dxfId="67" priority="107" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC34">
+  <conditionalFormatting sqref="AC23">
     <cfRule type="cellIs" dxfId="66" priority="106" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC23">
+  <conditionalFormatting sqref="AC25">
     <cfRule type="cellIs" dxfId="65" priority="105" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC25">
+  <conditionalFormatting sqref="AF48">
     <cfRule type="cellIs" dxfId="64" priority="104" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
@@ -8917,278 +8915,278 @@
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF48">
-    <cfRule type="cellIs" dxfId="62" priority="102" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W70">
-    <cfRule type="cellIs" dxfId="61" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="96" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA36 W36">
+    <cfRule type="cellIs" dxfId="61" priority="93" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X36:Y36 AJ36:AN36">
     <cfRule type="cellIs" dxfId="60" priority="92" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X36:Y36 AJ36:AN36">
+  <conditionalFormatting sqref="AF36">
     <cfRule type="cellIs" dxfId="59" priority="91" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF36">
+  <conditionalFormatting sqref="AG36:AI36">
     <cfRule type="cellIs" dxfId="58" priority="90" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG36:AI36">
+  <conditionalFormatting sqref="Z36:AB36">
     <cfRule type="cellIs" dxfId="57" priority="89" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z36:AB36">
-    <cfRule type="cellIs" dxfId="56" priority="88" operator="equal">
+  <conditionalFormatting sqref="B57:B60">
+    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:B60">
+  <conditionalFormatting sqref="AO60 AJ58:AN58">
     <cfRule type="cellIs" dxfId="55" priority="83" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO60 AJ58:AN58">
-    <cfRule type="cellIs" dxfId="54" priority="82" operator="equal">
+  <conditionalFormatting sqref="W62">
+    <cfRule type="cellIs" dxfId="54" priority="75" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W62">
+  <conditionalFormatting sqref="W66">
     <cfRule type="cellIs" dxfId="53" priority="74" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W66">
-    <cfRule type="cellIs" dxfId="52" priority="73" operator="equal">
+  <conditionalFormatting sqref="H5:H11 G8">
+    <cfRule type="cellIs" dxfId="52" priority="66" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:H11 G8">
+  <conditionalFormatting sqref="AF40">
     <cfRule type="cellIs" dxfId="51" priority="65" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF40">
+  <conditionalFormatting sqref="AF44">
     <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF44">
+  <conditionalFormatting sqref="B12:G13">
     <cfRule type="cellIs" dxfId="49" priority="63" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:G13">
+  <conditionalFormatting sqref="H12:H13">
     <cfRule type="cellIs" dxfId="48" priority="62" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H13">
-    <cfRule type="cellIs" dxfId="47" priority="61" operator="equal">
+  <conditionalFormatting sqref="W21:Y21 AA21:AY21">
+    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W21:Y21 AA21:AY21">
+  <conditionalFormatting sqref="Z21">
     <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z21">
-    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
+  <conditionalFormatting sqref="W38:Y38 AA38:AY38">
+    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W38:Y38 AA38:AY38">
+  <conditionalFormatting sqref="Z38">
     <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z38">
+  <conditionalFormatting sqref="W42:Y42 AA42:AY42">
     <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W42:Y42 AA42:AY42">
+  <conditionalFormatting sqref="Z42">
     <cfRule type="cellIs" dxfId="42" priority="53" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z42">
+  <conditionalFormatting sqref="W46:Y46 AA46:AY46">
     <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W46:Y46 AA46:AY46">
+  <conditionalFormatting sqref="Z46">
     <cfRule type="cellIs" dxfId="40" priority="51" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="39" priority="50" operator="equal">
+  <conditionalFormatting sqref="AB14:AY14">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB14:AY14">
+  <conditionalFormatting sqref="AA14">
     <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA14">
+  <conditionalFormatting sqref="I6:J13">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I6:J13">
+  <conditionalFormatting sqref="I5:J5">
     <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:J5">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+  <conditionalFormatting sqref="AR12:AY12 AO13:AY13">
+    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR12:AY12 AO13:AY13">
+  <conditionalFormatting sqref="AO11">
     <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO11">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+  <conditionalFormatting sqref="AF10:AN11 AF8:AQ9 AF7:AN7 AR5:AY11">
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AN11 AF8:AQ9 AF7:AN7 AR5:AY11">
-    <cfRule type="cellIs" dxfId="32" priority="35" operator="equal">
+  <conditionalFormatting sqref="AO29:AT29 AR27:AY27 W27:AE27 AA28:AE28 AF27:AN28 W31:AN31 AR31:AY31 AY28 AR28:AT28">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO28:AT29 AR27:AY27 W27:AE27 AA28:AE28 AF27:AN28 W31:AN31 AR31:AY31 AY28">
+  <conditionalFormatting sqref="AU28:AY29 AO30 W28:Y28">
     <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU28:AY29 AO30 W28:Y28">
+  <conditionalFormatting sqref="Z28">
     <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z28">
+  <conditionalFormatting sqref="W32:Y32 AA32:AY32">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W32:Y32 AA32:AY32">
+  <conditionalFormatting sqref="Z32">
     <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z32">
+  <conditionalFormatting sqref="AO50:AT51 AR49:AY49 W49:AE49 AA50:AE50 AF49:AN50 W53:AN53 AR53:AY53 AY50">
     <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO50:AT51 AR49:AY49 W49:AE49 AA50:AE50 AF49:AN50 W53:AN53 AR53:AY53 AY50">
+  <conditionalFormatting sqref="AU50:AY51 AO52 W50:Y50">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AU50:AY51 AO52 W50:Y50">
+  <conditionalFormatting sqref="Z50">
     <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z50">
+  <conditionalFormatting sqref="W54:Y54 AA54:AY54">
     <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W54:Y54 AA54:AY54">
+  <conditionalFormatting sqref="Z54">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z54">
+  <conditionalFormatting sqref="AS15">
     <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS15">
+  <conditionalFormatting sqref="AS23">
     <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS23">
+  <conditionalFormatting sqref="AS40">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS40">
+  <conditionalFormatting sqref="AS44">
     <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS44">
+  <conditionalFormatting sqref="AS48">
     <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AS48">
+  <conditionalFormatting sqref="N15">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N15">
+  <conditionalFormatting sqref="N23">
     <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N23">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N44">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N64">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O64:O67 O69:O75 O56:O59 O61:O62 O21:O29 O32:O54 O5:O18">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO28">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11054,37 +11052,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE9:XFD10 W11 AI15:XFD21 F29:XFD29 E9:V9 N30:XFD31 M29:M31 E22:XFD28 E18:V18 E21:AH21 E16:AH17 E30:E31 G30:L31 E12:XFD14 E4:XFD8 A10:B10 A21:C31 A12:C18 A4:C9 A19:B19">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:AD10">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE18:AH19 W20 E15:F15 Q15:AH15 H15:M15">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W18:AD19">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:P15">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
CI & input sheet updates
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model - Pole - Timber.xlsx
+++ b/data/inputs/Asset Model - Pole - Timber.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkirton1\OneDrive - KPMG\Documents\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D28E63D-327A-402D-98CF-50A2E87A6ACD}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{EF83B072-C8C0-4A7E-9BC1-52378010A04C}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1822,7 +1822,21 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{FE42BDC6-EBD5-43A7-A342-17D1DCC45724}"/>
   </cellStyles>
-  <dxfs count="103">
+  <dxfs count="105">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3327,7 +3341,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O13:O15 O17:O18">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3797,8 +3811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:AY78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -3809,39 +3823,42 @@
     <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="13.109375" customWidth="1"/>
     <col min="9" max="9" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="11.6640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="138" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.109375" style="159" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="6" style="162" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="6.88671875" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="132" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="138" customWidth="1"/>
+    <col min="14" max="14" width="12.109375" style="159" customWidth="1"/>
+    <col min="15" max="15" width="6" style="162" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" customWidth="1"/>
+    <col min="17" max="17" width="6.88671875" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" style="132" customWidth="1"/>
     <col min="19" max="19" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" style="98" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.5546875" customWidth="1"/>
+    <col min="24" max="24" width="11.109375" customWidth="1"/>
+    <col min="25" max="25" width="8.88671875" customWidth="1"/>
+    <col min="26" max="26" width="14.88671875" customWidth="1"/>
+    <col min="27" max="27" width="10.33203125" customWidth="1"/>
     <col min="28" max="28" width="14.88671875" customWidth="1"/>
-    <col min="29" max="29" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.6640625" customWidth="1"/>
+    <col min="30" max="30" width="8.88671875" customWidth="1"/>
+    <col min="31" max="31" width="9.5546875" customWidth="1"/>
     <col min="32" max="32" width="23.5546875" style="98" customWidth="1"/>
-    <col min="33" max="33" width="12" hidden="1" customWidth="1"/>
-    <col min="34" max="35" width="11.5546875" hidden="1" customWidth="1"/>
-    <col min="36" max="39" width="9.109375" style="17"/>
-    <col min="40" max="40" width="9.109375" style="111"/>
-    <col min="41" max="41" width="17.88671875" style="88" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.44140625" style="122" bestFit="1" customWidth="1"/>
-    <col min="44" max="45" width="9.109375" style="17"/>
-    <col min="46" max="46" width="9.109375" style="111"/>
-    <col min="47" max="47" width="17.88671875" style="77" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="9.109375" style="20"/>
-    <col min="49" max="49" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12" customWidth="1"/>
+    <col min="34" max="35" width="11.5546875" customWidth="1"/>
+    <col min="36" max="39" width="8.88671875" style="17" customWidth="1"/>
+    <col min="40" max="40" width="8.88671875" style="111" customWidth="1"/>
+    <col min="41" max="41" width="17.88671875" style="88" customWidth="1"/>
+    <col min="42" max="42" width="14.109375" style="20" customWidth="1"/>
+    <col min="43" max="43" width="14.44140625" style="122" customWidth="1"/>
+    <col min="44" max="45" width="8.88671875" style="17" customWidth="1"/>
+    <col min="46" max="46" width="8.88671875" style="111" customWidth="1"/>
+    <col min="47" max="47" width="17.88671875" style="77" customWidth="1"/>
+    <col min="48" max="48" width="8.88671875" style="20" customWidth="1"/>
+    <col min="49" max="49" width="16.33203125" customWidth="1"/>
+    <col min="50" max="50" width="8.88671875" customWidth="1"/>
     <col min="51" max="51" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4859,7 +4876,9 @@
       <c r="AG13" s="15"/>
       <c r="AH13" s="15"/>
       <c r="AI13" s="15"/>
-      <c r="AJ13" s="16"/>
+      <c r="AJ13" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK13" s="16"/>
       <c r="AL13" s="16" t="b">
         <v>1</v>
@@ -5331,7 +5350,9 @@
       <c r="AG21" s="15"/>
       <c r="AH21" s="15"/>
       <c r="AI21" s="15"/>
-      <c r="AJ21" s="16"/>
+      <c r="AJ21" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK21" s="16"/>
       <c r="AL21" s="16" t="b">
         <v>1</v>
@@ -5993,7 +6014,9 @@
       <c r="AG32" s="15"/>
       <c r="AH32" s="15"/>
       <c r="AI32" s="15"/>
-      <c r="AJ32" s="16"/>
+      <c r="AJ32" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK32" s="16"/>
       <c r="AL32" s="16" t="b">
         <v>1</v>
@@ -6393,7 +6416,9 @@
       <c r="AG38" s="15"/>
       <c r="AH38" s="15"/>
       <c r="AI38" s="15"/>
-      <c r="AJ38" s="16"/>
+      <c r="AJ38" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK38" s="16"/>
       <c r="AL38" s="16" t="b">
         <v>1</v>
@@ -6639,7 +6664,9 @@
       <c r="AG42" s="15"/>
       <c r="AH42" s="15"/>
       <c r="AI42" s="15"/>
-      <c r="AJ42" s="16"/>
+      <c r="AJ42" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK42" s="16"/>
       <c r="AL42" s="16" t="b">
         <v>1</v>
@@ -6905,7 +6932,9 @@
       <c r="AG46" s="15"/>
       <c r="AH46" s="15"/>
       <c r="AI46" s="15"/>
-      <c r="AJ46" s="16"/>
+      <c r="AJ46" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK46" s="16"/>
       <c r="AL46" s="16" t="b">
         <v>1</v>
@@ -7383,7 +7412,9 @@
       <c r="AG54" s="15"/>
       <c r="AH54" s="15"/>
       <c r="AI54" s="15"/>
-      <c r="AJ54" s="16"/>
+      <c r="AJ54" s="16" t="b">
+        <v>1</v>
+      </c>
       <c r="AK54" s="16"/>
       <c r="AL54" s="16" t="b">
         <v>1</v>
@@ -8716,477 +8747,487 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B7:B11 AA15 C21:D21 E20:H21 B65:B68 B14:B21 C16:D18 E15:H17 C7:G7 AG48:AR48 AO17:AT18 AR37:AT37 AR16:AY16 AR45:AY45 AR41:AY41 AR24:AY26 AR35:AT35 AU35:AY37 AO66:AY67 AR65:AY65 AO70:AY70 AR69:AY69 AO58:AY59 AR57:AY57 AO62:AY62 AR61:AY61 S35:V38 S46:V46 S69:V70 S59:V59 S32:V32 S27:V29 S74:X75 S25:AB25 B5:G6 AO36:AT36 S40:V42 B33:H54 AC15:AF15 W16:AE16 W69:AE69 W65:AE65 W35:AN35 W61:AE61 Z74:AE75 AB22:AX22 S26:AE26 AF58:AI58 S24:AN24 S57:AE58 AF57:AN57 AY57:AY58 S71:AE73 AF71:AX75 S33:AX33 S43:AX43 AF47:AX47 S39:AX39 AD34:AT34 AA17:AE17 AF16:AN17 W20:AN20 W37:AN37 S45:AN45 W41:AN41 AD23:AF23 AD25:AE25 AF25:AQ26 AR20:AY20 X66:AE66 AF65:AN66 AY64:AY66 X70:AE70 AF69:AN70 AY69:AY75 AC36:AF36 X62:AE62 AF61:AN62 AY61:AY62 C9:G11 C8:F8 W40:AB40 S47:AE48 AD40:AR40 AD44:AR44 AY22:AY26 AY33:AY37 AY39:AY41 AY43:AY45 AY47:AY48 AY15:AY17 C22:H23 B56:N56 B64:N64 AJ15:AR15 AT15:AY15 AJ23:AR23 AT23:AY23 AT40 AT44 AT48 P15:W15 P23:W23 P34:AB34 P44:AB44 P56:AY56 P64:AX64 P21:V21 I21:N29 P16:V18 I16:N18 P32:R33 I32:N54 P22:Z22 P65:V67 C65:N67 P69:R75 B69:N75 P57:R59 C57:N59 P61:V62 B61:N62 P24:R29 P35:R43 P45:R48 P49:V54 P14:Z14 C14:N15 P12:AN13 K5:N13 P7:AE11 P5:AQ6">
-    <cfRule type="cellIs" dxfId="102" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="250" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X15:Y15">
+    <cfRule type="cellIs" dxfId="103" priority="248" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF15">
+    <cfRule type="cellIs" dxfId="102" priority="246" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG15:AI15">
     <cfRule type="cellIs" dxfId="101" priority="245" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF15">
-    <cfRule type="cellIs" dxfId="100" priority="243" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG15:AI15">
-    <cfRule type="cellIs" dxfId="99" priority="242" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Z15:AB15">
-    <cfRule type="cellIs" dxfId="98" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="244" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X33:Z33">
+    <cfRule type="cellIs" dxfId="99" priority="238" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X34:Y34">
+    <cfRule type="cellIs" dxfId="98" priority="237" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF34">
     <cfRule type="cellIs" dxfId="97" priority="235" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X34:Y34">
+  <conditionalFormatting sqref="AG34:AI34">
     <cfRule type="cellIs" dxfId="96" priority="234" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF34">
-    <cfRule type="cellIs" dxfId="95" priority="232" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG34:AI34">
-    <cfRule type="cellIs" dxfId="94" priority="231" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="Z34:AB34">
-    <cfRule type="cellIs" dxfId="93" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="233" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU34:AY34">
-    <cfRule type="cellIs" dxfId="92" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="228" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU17:AY18 AO19 W17:Y17">
-    <cfRule type="cellIs" dxfId="91" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="218" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X44:Y44">
-    <cfRule type="cellIs" dxfId="90" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="199" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF44">
-    <cfRule type="cellIs" dxfId="89" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="198" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG44:AI44">
-    <cfRule type="cellIs" dxfId="88" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="197" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z44:AB44">
-    <cfRule type="cellIs" dxfId="87" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="196" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU44:AY44">
-    <cfRule type="cellIs" dxfId="86" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="193" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X48:Y48">
+    <cfRule type="cellIs" dxfId="87" priority="181" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG48:AI48">
+    <cfRule type="cellIs" dxfId="86" priority="179" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z48:AB48">
     <cfRule type="cellIs" dxfId="85" priority="178" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AG48:AI48">
-    <cfRule type="cellIs" dxfId="84" priority="176" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z48:AB48">
-    <cfRule type="cellIs" dxfId="83" priority="175" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AU48:AY48">
-    <cfRule type="cellIs" dxfId="82" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="175" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X40:Y40">
-    <cfRule type="cellIs" dxfId="81" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="163" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF40">
-    <cfRule type="cellIs" dxfId="80" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="162" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG40:AI40">
-    <cfRule type="cellIs" dxfId="79" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="161" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z40:AB40">
-    <cfRule type="cellIs" dxfId="78" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="160" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU40:AY40">
-    <cfRule type="cellIs" dxfId="77" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="157" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA22:AA23 B22:B32 C24:D29 E24:H28 C32:D32 E31:H32">
-    <cfRule type="cellIs" dxfId="76" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="147" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23:Y23">
-    <cfRule type="cellIs" dxfId="75" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="146" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF23">
-    <cfRule type="cellIs" dxfId="74" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="145" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG23:AI23">
-    <cfRule type="cellIs" dxfId="73" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="144" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23:AB23">
-    <cfRule type="cellIs" dxfId="72" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="143" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO68">
-    <cfRule type="cellIs" dxfId="71" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="123" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z17">
-    <cfRule type="cellIs" dxfId="70" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="113" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC44">
-    <cfRule type="cellIs" dxfId="69" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="112" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC40">
-    <cfRule type="cellIs" dxfId="68" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="111" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC34">
-    <cfRule type="cellIs" dxfId="67" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="110" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC23">
-    <cfRule type="cellIs" dxfId="66" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="109" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC25">
-    <cfRule type="cellIs" dxfId="65" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="108" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF48">
-    <cfRule type="cellIs" dxfId="64" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="107" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF48">
-    <cfRule type="cellIs" dxfId="63" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="106" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W70">
-    <cfRule type="cellIs" dxfId="62" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="99" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA36 W36">
-    <cfRule type="cellIs" dxfId="61" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="96" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X36:Y36 AJ36:AN36">
-    <cfRule type="cellIs" dxfId="60" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="95" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF36">
-    <cfRule type="cellIs" dxfId="59" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="94" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG36:AI36">
-    <cfRule type="cellIs" dxfId="58" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="93" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z36:AB36">
-    <cfRule type="cellIs" dxfId="57" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="92" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B60">
-    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="87" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO60 AJ58:AN58">
-    <cfRule type="cellIs" dxfId="55" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="86" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W62">
-    <cfRule type="cellIs" dxfId="54" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="78" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W66">
-    <cfRule type="cellIs" dxfId="53" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="77" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H11 G8">
-    <cfRule type="cellIs" dxfId="52" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF40">
-    <cfRule type="cellIs" dxfId="51" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="68" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF44">
-    <cfRule type="cellIs" dxfId="50" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="67" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:G13">
+    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H13">
+    <cfRule type="cellIs" dxfId="50" priority="65" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W21:Y21 AA21:AY21">
     <cfRule type="cellIs" dxfId="49" priority="63" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H13">
+  <conditionalFormatting sqref="Z21">
     <cfRule type="cellIs" dxfId="48" priority="62" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="W21:Y21 AA21:AY21">
-    <cfRule type="cellIs" dxfId="47" priority="60" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z21">
-    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="W38:Y38 AA38:AY38">
-    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="59" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z38">
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="58" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W42:Y42 AA42:AY42">
-    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z42">
-    <cfRule type="cellIs" dxfId="42" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W46:Y46 AA46:AY46">
-    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="55" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="40" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB14:AY14">
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J13">
+    <cfRule type="cellIs" dxfId="39" priority="41" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5:J5">
+    <cfRule type="cellIs" dxfId="38" priority="40" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR12:AY12 AO13:AY13">
     <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:J5">
+  <conditionalFormatting sqref="AO11">
     <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR12:AY12 AO13:AY13">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+  <conditionalFormatting sqref="AF10:AN11 AF8:AQ9 AF7:AN7 AR5:AY11">
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO11">
+  <conditionalFormatting sqref="AR27:AY27 W27:AE27 AA28:AE28 AF27:AN28 W31:AN31 AR31:AY31 AY28 AR28:AT29">
     <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF10:AN11 AF8:AQ9 AF7:AN7 AR5:AY11">
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO29:AT29 AR27:AY27 W27:AE27 AA28:AE28 AF27:AN28 W31:AN31 AR31:AY31 AY28 AR28:AT28">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
-      <formula>"nil"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU28:AY29 AO30 W28:Y28">
-    <cfRule type="cellIs" dxfId="31" priority="30" operator="equal">
+  <conditionalFormatting sqref="AU28:AY29 W28:Y28">
+    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z28">
-    <cfRule type="cellIs" dxfId="30" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W32:Y32 AA32:AY32">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z32">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO50:AT51 AR49:AY49 W49:AE49 AA50:AE50 AF49:AN50 W53:AN53 AR53:AY53 AY50">
-    <cfRule type="cellIs" dxfId="27" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU50:AY51 AO52 W50:Y50">
-    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z50">
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W54:Y54 AA54:AY54">
-    <cfRule type="cellIs" dxfId="24" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z54">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS15">
-    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS23">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS40">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS44">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS48">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N23">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N56">
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N44">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N34">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N64">
-    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="11" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N48">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N40">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O64:O67 O69:O75 O56:O59 O61:O62 O21:O29 O32:O54 O5:O18">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO30">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+      <formula>"nil"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO29:AQ29">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO28">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11052,37 +11093,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE9:XFD10 W11 AI15:XFD21 F29:XFD29 E9:V9 N30:XFD31 M29:M31 E22:XFD28 E18:V18 E21:AH21 E16:AH17 E30:E31 G30:L31 E12:XFD14 E4:XFD8 A10:B10 A21:C31 A12:C18 A4:C9 A19:B19">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:AD10">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE18:AH19 W20 E15:F15 Q15:AH15 H15:M15">
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W18:AD19">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:P15">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>